<commit_message>
Import file excel from FE
</commit_message>
<xml_diff>
--- a/Resource/TestExcel/Test.xlsx
+++ b/Resource/TestExcel/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\TestExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\MISA-CukCuk-Duplicate\Resource\TestExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3DE398-BAD6-4AC1-BDFF-28162F94225B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75101D6-D89C-47FE-83A0-B5831452CB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E032AE7C-7CB2-4D49-BBEC-605C9B1576C3}"/>
+    <workbookView xWindow="60" yWindow="1965" windowWidth="21600" windowHeight="11385" xr2:uid="{E032AE7C-7CB2-4D49-BBEC-605C9B1576C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Mã nguyên vật liệu</t>
   </si>
@@ -64,9 +64,6 @@
     <t>BH-60813</t>
   </si>
   <si>
-    <t>BH-60812</t>
-  </si>
-  <si>
     <t>BH-60811</t>
   </si>
   <si>
@@ -77,12 +74,6 @@
   </si>
   <si>
     <t>Bia Hơi</t>
-  </si>
-  <si>
-    <t>Bia có ga</t>
-  </si>
-  <si>
-    <t>Bia có cồn</t>
   </si>
   <si>
     <t>Bia không cồn</t>
@@ -516,7 +507,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,16 +542,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -568,22 +559,20 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -591,17 +580,15 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -609,74 +596,72 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>